<commit_message>
Them kich ban test thu cong
</commit_message>
<xml_diff>
--- a/_Kich ban test.xlsx
+++ b/_Kich ban test.xlsx
@@ -8,12 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Codes\mincloset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE69465-99DC-43CA-B021-3E54312D507F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7448B8A2-EBC5-4EB3-A6FF-3F33F2589EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="Closet" sheetId="1" r:id="rId1"/>
+    <sheet name="Item" sheetId="3" r:id="rId2"/>
+    <sheet name="Outfit Builder" sheetId="4" r:id="rId3"/>
+    <sheet name="AI" sheetId="6" r:id="rId4"/>
+    <sheet name="Journal" sheetId="8" r:id="rId5"/>
+    <sheet name="Profile" sheetId="9" r:id="rId6"/>
+    <sheet name="Settings" sheetId="10" r:id="rId7"/>
+    <sheet name="Quests" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="188">
   <si>
     <t>ID</t>
   </si>
@@ -45,13 +52,7 @@
     <t>Kết quả mong đợi</t>
   </si>
   <si>
-    <t>Kết quả thực tế</t>
-  </si>
-  <si>
     <t>CLO-001</t>
-  </si>
-  <si>
-    <t>Quản lý Tủ đồ</t>
   </si>
   <si>
     <t>CLO-002</t>
@@ -181,12 +182,583 @@
     <t>1. Một banner lỗi "Đã đạt giới hạn số lượng tủ đồ (10)" hiển thị.
 2. Màn hình Thêm Tủ đồ không đóng lại.</t>
   </si>
+  <si>
+    <t>ITEM-001</t>
+  </si>
+  <si>
+    <t>Quản lý Vật phẩm</t>
+  </si>
+  <si>
+    <t>Thêm một vật phẩm mới thành công với phân loại AI</t>
+  </si>
+  <si>
+    <t>Đã có ít nhất một tủ đồ.</t>
+  </si>
+  <si>
+    <t>ITEM-002</t>
+  </si>
+  <si>
+    <t>Thêm nhiều vật phẩm mới thành công (batch add)</t>
+  </si>
+  <si>
+    <t>ITEM-003</t>
+  </si>
+  <si>
+    <t>Sửa thông tin chi tiết của một vật phẩm</t>
+  </si>
+  <si>
+    <t>Đã có một vật phẩm trong tủ đồ.</t>
+  </si>
+  <si>
+    <t>ITEM-004</t>
+  </si>
+  <si>
+    <t>Xóa một vật phẩm thành công</t>
+  </si>
+  <si>
+    <t>ITEM-005</t>
+  </si>
+  <si>
+    <t>Di chuyển nhiều vật phẩm sang một tủ đồ khác</t>
+  </si>
+  <si>
+    <t>Có ít nhất 2 tủ đồ (Closet A, Closet B). Closet A có ít nhất 2 vật phẩm.</t>
+  </si>
+  <si>
+    <t>ITEM-006</t>
+  </si>
+  <si>
+    <t>Thêm vật phẩm thất bại do thiếu trường bắt buộc</t>
+  </si>
+  <si>
+    <t>ITEM-007</t>
+  </si>
+  <si>
+    <t>Lọc vật phẩm theo danh mục và màu sắc</t>
+  </si>
+  <si>
+    <t>Có nhiều vật phẩm với danh mục và màu sắc khác nhau.</t>
+  </si>
+  <si>
+    <t>Chỉ những vật phẩm là Tops và có màu White được hiển thị trong danh sách.</t>
+  </si>
+  <si>
+    <t>1. Từ Home, nhấn nút Add Item và chọn From album.
+2. Chọn một ảnh áo sơ mi.
+3. Chờ màn hình Analysis Loading hoàn tất.
+4. Tại màn hình Add Item, kiểm tra các trường Item name, Category đã được AI điền trước.
+5. Chọn một tủ đồ từ dropdown Select closet.
+6. Nhấn Save.</t>
+  </si>
+  <si>
+    <t>1. Màn hình điều hướng về tab Closets -&gt; All Items.
+2. Vật phẩm áo sơ mi mới xuất hiện đầu danh sách.
+3. Một banner thông báo thành công hiển thị.</t>
+  </si>
+  <si>
+    <t>1. Từ Home, nhấn nút Add Item và chọn From album.
+2. Chọn 3 ảnh khác nhau.
+3. Chờ màn hình Analysis Loading hoàn tất.
+4. Tại màn hình Add item (1/3), điền/chỉnh sửa thông tin và nhấn Next.
+5. Lặp lại cho item 2/3.
+6. Tại màn hình Add item (3/3), điền thông tin và nhấn Save all.</t>
+  </si>
+  <si>
+    <t>1. Màn hình điều hướng về tab Closets -&gt; All Items.
+2. Cả 3 vật phẩm mới đều xuất hiện trong danh sách.
+3. Một banner thông báo thành công hiển thị.</t>
+  </si>
+  <si>
+    <t>1. Điều hướng đến tab Closets -&gt; All Items.
+2. Nhấn vào một vật phẩm để mở màn hình Edit item.
+3. Thay đổi Item name, Category, và thêm một Note.
+4. Nhấn Save.</t>
+  </si>
+  <si>
+    <t>1. Màn hình điều hướng về trang trước đó.
+2. Một banner thông báo cập nhật thành công hiển thị.
+3. (Kiểm tra lại) Mở lại chi tiết vật phẩm, các thông tin đã thay đổi được lưu chính xác.</t>
+  </si>
+  <si>
+    <t>1. Điều hướng đến tab Closets -&gt; All Items.
+2. Nhấn vào một vật phẩm để mở màn hình Edit item.
+3. Nhấn vào icon thùng rác ở góc trên bên phải.
+4. Trong dialog xác nhận, nhấn Delete.</t>
+  </si>
+  <si>
+    <t>1. Màn hình điều hướng về trang trước đó.
+2. Vật phẩm đã chọn biến mất khỏi danh sách.
+3. Một banner thông báo xóa thành công hiển thị.</t>
+  </si>
+  <si>
+    <t>1. Điều hướng đến Closet A.
+2. Nhấn giữ một vật phẩm để kích hoạt chế độ đa chọn.
+3. Chọn thêm một vật phẩm nữa (tổng cộng 2).
+4. Nhấn nút Move ở thanh dưới cùng.
+5. Trong dialog, chọn Closet B.</t>
+  </si>
+  <si>
+    <t>1. Các vật phẩm đã chọn biến mất khỏi Closet A.
+2. Điều hướng sang Closet B, hai vật phẩm đã chọn xuất hiện ở đó.
+3. Một banner thông báo di chuyển thành công hiển thị.</t>
+  </si>
+  <si>
+    <t>1. Mở màn hình Add Item với một ảnh.
+2. Nhập Item name.
+3. Không chọn tủ đồ (Select closet).
+4. Nhấn Save.</t>
+  </si>
+  <si>
+    <t>1. Một banner lỗi "Please select a closet" hiển thị.
+2. Màn hình Add Item không đóng lại.</t>
+  </si>
+  <si>
+    <t>1. Điều hướng đến tab Closets -&gt; All Items.
+2. Nhấn vào icon Filter.
+3. Trong Category, chọn Tops.
+4. Trong Color, chọn White.
+5. Nhấn Apply.</t>
+  </si>
+  <si>
+    <t>OUTFIT-001</t>
+  </si>
+  <si>
+    <t>Tạo và lưu outfit mới thành công</t>
+  </si>
+  <si>
+    <t>Có ít nhất 2 vật phẩm trong tủ đồ.</t>
+  </si>
+  <si>
+    <t>OUTFIT-002</t>
+  </si>
+  <si>
+    <t>Tạo outfit từ các vật phẩm đã chọn trước</t>
+  </si>
+  <si>
+    <t>Đã có ít nhất 2 vật phẩm.</t>
+  </si>
+  <si>
+    <t>OUTFIT-003</t>
+  </si>
+  <si>
+    <t>Thay đổi ảnh nền thành công</t>
+  </si>
+  <si>
+    <t>Đang ở trong màn hình Outfit studio.</t>
+  </si>
+  <si>
+    <t>1. Ảnh nền của canvas được thay thế bằng ảnh vừa chọn và cắt.</t>
+  </si>
+  <si>
+    <t>OUTFIT-004</t>
+  </si>
+  <si>
+    <t>Lưu outfit thất bại do không nhập tên</t>
+  </si>
+  <si>
+    <t>Đang ở trong màn hình Outfit studio với ít nhất 1 vật phẩm trên canvas.</t>
+  </si>
+  <si>
+    <t>OUTFIT-005</t>
+  </si>
+  <si>
+    <t>Lưu outfit thất bại do không có vật phẩm</t>
+  </si>
+  <si>
+    <t>OUTFIT-006</t>
+  </si>
+  <si>
+    <t>Lưu "Fixed outfit" thất bại do vật phẩm bị trùng</t>
+  </si>
+  <si>
+    <t>- Đã có một "Fixed outfit" tên "Set A" chứa "Áo sơ mi trắng".- Đang ở Outfit studio với "Áo sơ mi trắng" và "Quần jean xanh" trên canvas.</t>
+  </si>
+  <si>
+    <t>1. Từ màn hình Home, điều hướng đến Create Outfits.
+2. Kéo 1 "Áo" và 1 "Quần" từ thanh vật phẩm vào canvas.
+3. Sắp xếp vị trí các vật phẩm.
+4. Nhấn nút Save.
+5. Trong dialog, nhập tên "Outfit dạo phố".
+6. Nhấn Save trong dialog.</t>
+  </si>
+  <si>
+    <t>1. Màn hình điều hướng về trang Outfits.
+2. Một thẻ outfit mới tên "Outfit dạo phố" xuất hiện đầu danh sách.
+3. Một banner thông báo lưu thành công hiển thị.</t>
+  </si>
+  <si>
+    <t>1. Từ tab Closets -&gt; All Items, nhấn giữ và chọn 2 vật phẩm.
+2. Nhấn nút Create Outfit ở thanh dưới cùng.
+3. Ứng dụng điều hướng đến màn hình Outfit studio.
+4. Nhấn Save.
+5. Nhập tên và nhấn Save trong dialog.</t>
+  </si>
+  <si>
+    <t>1. Hai vật phẩm đã chọn phải có sẵn trên canvas khi màn hình Outfit studio mở ra.
+2. Luồng lưu outfit hoạt động thành công như kịch bản OUTFIT-001.</t>
+  </si>
+  <si>
+    <t>1. Nhấn nút Change background.
+2. Chọn một ảnh từ thư viện.
+3. Cắt (crop) ảnh theo tỷ lệ 3:4.
+4. Nhấn Done.</t>
+  </si>
+  <si>
+    <t>1. Nhấn nút Save.
+2. Trong dialog, không nhập gì vào ô tên.
+3. Nhấn Save trong dialog.</t>
+  </si>
+  <si>
+    <t>1. Hiển thị thông báo lỗi "Please enter an outfit name" ngay dưới ô nhập liệu.
+2. Dialog không đóng lại.</t>
+  </si>
+  <si>
+    <t>1. Đảm bảo không có vật phẩm nào trên canvas.
+2. Nhấn nút Save.
+3. Trong dialog, nhập tên hợp lệ.
+4. Nhấn Save trong dialog.</t>
+  </si>
+  <si>
+    <t>1. Một banner lỗi "Please add at least one item to save the outfit!" hiển thị.
+2. Màn hình Outfit studio không đóng lại.</t>
+  </si>
+  <si>
+    <t>1. Nhấn nút Save.
+2. Nhập tên "Set B".
+3. Gạt nút Fixed outfit sang BẬT.
+4. Nhấn Save trong dialog.</t>
+  </si>
+  <si>
+    <t>1. Một banner lỗi hiển thị, ví dụ: "Error: 'Áo sơ mi trắng' already belongs to another fixed outfit."
+2. Màn hình Outfit studio không đóng lại.</t>
+  </si>
+  <si>
+    <t>AI-001</t>
+  </si>
+  <si>
+    <t>Gợi ý AI</t>
+  </si>
+  <si>
+    <t>Nhận gợi ý trang phục thành công</t>
+  </si>
+  <si>
+    <t>AI-002</t>
+  </si>
+  <si>
+    <t>Lưu lại một trang phục được gợi ý</t>
+  </si>
+  <si>
+    <t>Đã nhận được một gợi ý trang phục thành công (sau khi thực hiện AI-001).</t>
+  </si>
+  <si>
+    <t>AI-003</t>
+  </si>
+  <si>
+    <t>Nhận gợi ý thất bại do không đủ vật phẩm</t>
+  </si>
+  <si>
+    <t>Người dùng có ít hơn 3 áo (Tops) hoặc 3 quần/váy (Bottoms).</t>
+  </si>
+  <si>
+    <t>1. Tại màn hình Home, nhập mục đích và nhấn nút Send.</t>
+  </si>
+  <si>
+    <t>AI-004</t>
+  </si>
+  <si>
+    <t>Xử lý lỗi khi không có kết nối mạng</t>
+  </si>
+  <si>
+    <t>Tắt Wifi và Dữ liệu di động trên thiết bị.</t>
+  </si>
+  <si>
+    <t>1. Tại màn hình Home, nhấn nút Send để nhận gợi ý.</t>
+  </si>
+  <si>
+    <t>AI-005</t>
+  </si>
+  <si>
+    <t>Xử lý lỗi khi người dùng từ chối quyền vị trí</t>
+  </si>
+  <si>
+    <t>1. Tại màn hình Home, nhập mục đích "Đi cà phê" vào ô Purpose.
+2. Nhấn nút Send (icon máy bay giấy).
+3. Chờ quá trình xử lý hoàn tất.</t>
+  </si>
+  <si>
+    <t>1. Một bộ trang phục hoàn chỉnh (gồm ảnh các vật phẩm) được hiển thị.
+2. Tên và lý do gợi ý được hiển thị bên dưới.
+3. Thông tin thời tiết được cập nhật chính xác.</t>
+  </si>
+  <si>
+    <t>1. Nhấn nút Edit &amp; Save bên dưới trang phục được gợi ý.
+2. Ứng dụng điều hướng đến màn hình Outfit studio.
+3. Nhấn nút Save.
+4. Trong dialog, giữ nguyên tên hoặc đổi tên mới.
+5. Nhấn Save trong dialog.</t>
+  </si>
+  <si>
+    <t>1. Các vật phẩm từ gợi ý được tự động đặt lên canvas của Outfit studio.
+2. Luồng lưu outfit hoạt động thành công như kịch bản OUTFIT-001.
+3. Trang phục được lưu vào danh sách Outfits.</t>
+  </si>
+  <si>
+    <t>1. Một banner lỗi hiển thị thông báo "Please add at least 3 tops and 3 bottoms/skirts to your closet to receive suggestions.".
+2. Khu vực gợi ý không thay đổi.</t>
+  </si>
+  <si>
+    <t>1. Một banner lỗi "Please check your internet connection." hiển thị.
+2. Khu vực gợi ý không thay đổi.</t>
+  </si>
+  <si>
+    <t>1. Mở lại ứng dụng và điều hướng đến màn hình Home.
+2. Nhấn nút Send để nhận gợi ý.</t>
+  </si>
+  <si>
+    <t>1. Một banner lỗi "Location permissions are denied..." hiển thị.
+2. Khu vực gợi ý không thay đổi.</t>
+  </si>
+  <si>
+    <t>1. Người dùng có ít nhất 3 áo (Tops) và 3 quần/váy (Bottoms).
+2. Kết nối mạng ổn định.
+3. Đã cấp quyền vị trí.</t>
+  </si>
+  <si>
+    <t>1. Trong cài đặt hệ thống, thu hồi quyền vị trí của ứng dụng MinCloset.
+2. Cài đặt vị trí trong app là Auto-detect.</t>
+  </si>
+  <si>
+    <t>Ghi lại một vật phẩm cho ngày hôm nay thành công</t>
+  </si>
+  <si>
+    <t>Ghi lại một trang phục cho một ngày trong quá khứ</t>
+  </si>
+  <si>
+    <t>Xóa một log vật phẩm bằng cách vuốt</t>
+  </si>
+  <si>
+    <t>Đã có một vật phẩm được ghi lại cho ngày hôm nay.</t>
+  </si>
+  <si>
+    <t>Xóa nhiều log cùng lúc bằng chế độ đa chọn</t>
+  </si>
+  <si>
+    <t>Đã có ít nhất 2 vật phẩm/trang phục được ghi lại cho ngày hôm nay.</t>
+  </si>
+  <si>
+    <t>Điều hướng đến chi tiết vật phẩm/trang phục từ lịch</t>
+  </si>
+  <si>
+    <t>Đã có một vật phẩm và một trang phục được ghi lại trên lịch.</t>
+  </si>
+  <si>
+    <t>Ghi log thất bại do không chọn gì</t>
+  </si>
+  <si>
+    <t>Đang ở màn hình Select Items hoặc Select Outfits.</t>
+  </si>
+  <si>
+    <t>1. Nhấn nút Save mà không chọn bất kỳ vật phẩm/trang phục nào.</t>
+  </si>
+  <si>
+    <t>Nút Save bị vô hiệu hóa (không thể nhấn).</t>
+  </si>
+  <si>
+    <t>1. Điều hướng đến CalendarPage.
+2. Nhấn nút Add.
+3. Chọn Select Items.
+4. Chọn một vật phẩm từ danh sách.
+5. Nhấn Save.</t>
+  </si>
+  <si>
+    <t>1. Có ít nhất một vật phẩm.
+2. Lịch của ngày hôm nay đang trống.</t>
+  </si>
+  <si>
+    <t>1. Một thẻ hiển thị vật phẩm đã chọn xuất hiện trong danh sách của ngày hôm nay.
+2. Trên ô lịch của ngày hôm nay, một chỉ báo (marker) hiển thị số lượng "1".</t>
+  </si>
+  <si>
+    <t>1. Có ít nhất một trang phục (outfit). 
+2. Lịch của ngày hôm qua đang trống.</t>
+  </si>
+  <si>
+    <t>1. Điều hướng đến CalendarPage.
+2. Chọn ngày hôm qua trên lịch.
+3. Nhấn nút Add.
+4. Chọn Select Outfits.
+5. Chọn một trang phục từ danh sách.
+6. Nhấn Save.</t>
+  </si>
+  <si>
+    <t>1. Một thẻ hiển thị trang phục đã chọn xuất hiện trong danh sách của ngày hôm qua.
+2. Trên ô lịch của ngày hôm qua, một chỉ báo hiển thị số lượng vật phẩm có trong trang phục đó.</t>
+  </si>
+  <si>
+    <t>1. Tại CalendarPage, vuốt sang trái trên thẻ vật phẩm của ngày hôm nay.
+2. Trong dialog xác nhận, nhấn Delete.</t>
+  </si>
+  <si>
+    <t>1. Thẻ vật phẩm biến mất khỏi danh sách.
+2. Chỉ báo trên ô lịch của ngày hôm nay biến mất hoặc giảm đi 1.</t>
+  </si>
+  <si>
+    <t>1. Tại CalendarPage, nhấn giữ một thẻ log để kích hoạt chế độ đa chọn.
+2. Chọn thêm một thẻ log khác.
+3. Nhấn vào icon thùng rác trên AppBar.
+4. Trong dialog xác nhận, nhấn Delete.</t>
+  </si>
+  <si>
+    <t>1. Cả hai thẻ đã chọn biến mất khỏi danh sách.
+2. Chỉ báo trên ô lịch được cập nhật chính xác.</t>
+  </si>
+  <si>
+    <t>1. Tại CalendarPage, nhấn vào thẻ log của một vật phẩm.
+2. Quay lại.
+3. Nhấn vào thẻ log của một trang phục.</t>
+  </si>
+  <si>
+    <t>1. Ứng dụng điều hướng đến màn hình Edit item tương ứng.
+2. Ứng dụng điều hướng đến màn hình Outfit Detail tương ứng.</t>
+  </si>
+  <si>
+    <t>JOU-001</t>
+  </si>
+  <si>
+    <t>JOU-002</t>
+  </si>
+  <si>
+    <t>JOU-003</t>
+  </si>
+  <si>
+    <t>JOU-004</t>
+  </si>
+  <si>
+    <t>JOU-005</t>
+  </si>
+  <si>
+    <t>JOU-006</t>
+  </si>
+  <si>
+    <t>Journal</t>
+  </si>
+  <si>
+    <t>Outfit Builder</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Closet</t>
+  </si>
+  <si>
+    <t>PRO-001</t>
+  </si>
+  <si>
+    <t>Sửa thông tin cá nhân thành công</t>
+  </si>
+  <si>
+    <t>Đang ở màn hình Profile.</t>
+  </si>
+  <si>
+    <t>SET-001</t>
+  </si>
+  <si>
+    <t>Thay đổi đơn vị đo lường thành công</t>
+  </si>
+  <si>
+    <t>SET-002</t>
+  </si>
+  <si>
+    <t>Thay đổi cài đặt hiển thị thành công</t>
+  </si>
+  <si>
+    <t>Đang ở màn hình Home.</t>
+  </si>
+  <si>
+    <t>QUEST-001</t>
+  </si>
+  <si>
+    <t>Hoàn thành nhiệm vụ "First Steps"</t>
+  </si>
+  <si>
+    <t>QUEST-002</t>
+  </si>
+  <si>
+    <t>Mở khóa thành tích "Beginner Quests"</t>
+  </si>
+  <si>
+    <t>Đã hoàn thành 4/5 nhiệm vụ tân thủ. Nhiệm vụ cuối cùng là "Track Your Style Journey".</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>1. Nhấn Edit profile.
+2. Nhập một Full name mới.
+3. Chọn một Gender khác.
+4. Chọn một Birthday.
+5. Nhấn Save.</t>
+  </si>
+  <si>
+    <t>1. Màn hình điều hướng về trang Profile.
+2. Tên người dùng trên AppBar và trong phần thông tin được cập nhật chính xác.</t>
+  </si>
+  <si>
+    <t>Cài đặt</t>
+  </si>
+  <si>
+    <t>1. Nhấn icon Settings.
+2. Mở mục Units.
+3. Thay đổi Height từ cm sang ft.
+4. Thay đổi Weight từ kg sang lbs.
+5. Quay lại màn hình Edit profile.</t>
+  </si>
+  <si>
+    <t>1. Điều hướng đến Settings -&gt; Display.
+2. Tắt tùy chọn Show weather background.
+3. Tắt tùy chọn Show Mascot.
+4. Quay lại màn hình Home.</t>
+  </si>
+  <si>
+    <t>1. Trong màn hình Edit profile, ô nhập liệu cho chiều cao chuyển thành 2 ô (feet và inches).
+2. Nhãn của ô cân nặng đổi thành "Weight (lbs)".</t>
+  </si>
+  <si>
+    <t>1. Ảnh nền thời tiết biến mất, thay bằng màu nền trơn.
+2. Mascot trợ lý biến mất khỏi màn hình.</t>
+  </si>
+  <si>
+    <t>Quests</t>
+  </si>
+  <si>
+    <t>1. Người dùng là tài khoản mới. 
+2. Đã có 2 áo và 3 quần/váy.</t>
+  </si>
+  <si>
+    <t>1. Thêm một vật phẩm Tops mới.
+2. Quan sát mascot.</t>
+  </si>
+  <si>
+    <t>1. Điều hướng đến CalendarPage.
+2. Ghi lại một vật phẩm bất kỳ cho ngày hôm nay.
+3. Quan sát màn hình.</t>
+  </si>
+  <si>
+    <t>1. Mascot hiển thị thông báo "Quest Completed!".
+2. Điều hướng vào Achievements, nhiệm vụ "First Steps" chuyển sang trạng thái hoàn thành.
+3. Nhiệm vụ "Your First AI-Powered Suggestion" được mở khóa và chuyển sang trạng thái "In Progress".</t>
+  </si>
+  <si>
+    <t>1. Một dialog "ACHIEVEMENT UNLOCKED!" hiển thị cùng với huy hiệu "Fashion Beginner".
+2. Trong trang Achievements, huy hiệu "Fashion Beginner" trở nên sáng màu (không bị làm mờ).</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +778,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -230,13 +808,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -521,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,156 +1133,1166 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73270A5B-C184-4FA4-8AB3-E66ABC5A3608}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="52.42578125" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="102" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="G8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BD1177-2369-4C81-9EC1-E65AA912F1C0}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="52.42578125" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="102" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5D33F4-A4BD-41F0-ABC2-86F1681510E3}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="52.42578125" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987B3FBF-0330-448F-895B-9993A9EBF093}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="52.42578125" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{918D4B43-9FE7-449D-B8CB-2D3AEB4D3185}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="52.42578125" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6BCE5A7-7713-4747-A50D-F4ABA0FAEA7C}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="52.42578125" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DA5B72-5280-417F-9482-D3860A78688B}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="52.42578125" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>